<commit_message>
change ogimet hora to 12
</commit_message>
<xml_diff>
--- a/气象/北境强冷站每日气温记录.xlsx
+++ b/气象/北境强冷站每日气温记录.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\GIT SYNC\default\气象\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192770D9-B99B-4676-B412-74C2C7AFEC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B11E574-A042-4F2F-B145-826EE7876255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{21DDB67E-D335-466F-8652-CD2F68303142}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
   <si>
     <t>漠河</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -511,7 +511,49 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11月15日</t>
+    <t>巴音郭楞乡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尧勒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三河马场五队</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三道海子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>蒙古国5个非国家站，早上8点看昨天夜里低温情况，顺带也记录昨夜高温情况。晚上8点看今天白天高温情况，低温可能出现在早8以后，所以晚上8点要再检查高低温一次。</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>同时还要考虑高低温不要和上一个24小时重复</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11月17日</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,7 +564,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,8 +711,41 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,8 +788,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA604"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -829,13 +910,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -920,32 +1047,56 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="19" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -955,10 +1106,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF8EA604"/>
       <color rgb="FF4CC9F0"/>
       <color rgb="FF480CA8"/>
       <color rgb="FFBF3100"/>
-      <color rgb="FF8EA604"/>
       <color rgb="FFEC9F05"/>
       <color rgb="FF3A0CA3"/>
       <color rgb="FFF72585"/>
@@ -1275,15 +1426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E72AAA-3912-4684-8CF1-D56A9EC12E76}">
-  <dimension ref="A1:AE25"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.59765625" style="36" customWidth="1"/>
+    <col min="1" max="1" width="20.59765625" style="31" customWidth="1"/>
     <col min="2" max="3" width="12.59765625" style="6" customWidth="1"/>
     <col min="4" max="6" width="8.59765625" style="6" customWidth="1"/>
     <col min="7" max="7" width="32.59765625" style="6" customWidth="1"/>
@@ -1291,290 +1442,260 @@
     <col min="9" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="10" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
+    </row>
+    <row r="2" spans="1:31" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F2" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="20">
-        <v>-27.5</v>
-      </c>
-      <c r="C2" s="20">
-        <v>-11.9</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" s="7" cm="1">
-        <f t="array" ref="H2:AE2">TRANSPOSE(B2:B25)</f>
-        <v>-27.5</v>
-      </c>
-      <c r="I2" s="7">
-        <v>-22.8</v>
-      </c>
-      <c r="J2" s="7">
-        <v>-26</v>
-      </c>
-      <c r="K2" s="7">
-        <v>6.7</v>
-      </c>
-      <c r="L2" s="7">
-        <v>-17.2</v>
-      </c>
-      <c r="M2" s="7">
-        <v>-14.3</v>
-      </c>
-      <c r="N2" s="7">
-        <v>-16</v>
-      </c>
-      <c r="O2" s="7">
-        <v>-13.2</v>
-      </c>
-      <c r="P2" s="7">
-        <v>-25.6</v>
-      </c>
-      <c r="Q2" s="7">
-        <v>-21.7</v>
-      </c>
-      <c r="R2" s="7">
-        <v>-19.2</v>
-      </c>
-      <c r="S2" s="7">
-        <v>-9.5</v>
-      </c>
-      <c r="T2" s="7">
-        <v>-9.6</v>
-      </c>
-      <c r="U2" s="7">
-        <v>-26.9</v>
-      </c>
-      <c r="V2" s="7">
-        <v>-11.7</v>
-      </c>
-      <c r="W2" s="7">
-        <v>-16.899999999999999</v>
-      </c>
-      <c r="X2" s="7">
-        <v>-12.7</v>
-      </c>
-      <c r="Y2" s="7">
-        <v>-15.5</v>
-      </c>
-      <c r="Z2" s="7">
-        <v>-18</v>
-      </c>
-      <c r="AA2" s="7">
-        <v>-20</v>
-      </c>
-      <c r="AB2" s="7">
-        <v>-23.5</v>
-      </c>
-      <c r="AC2" s="7">
-        <v>-25.5</v>
-      </c>
-      <c r="AD2" s="7">
-        <v>-14.4</v>
-      </c>
-      <c r="AE2" s="7">
-        <v>-24.1</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="20">
-        <v>-22.8</v>
-      </c>
-      <c r="C3" s="20">
-        <v>-5.6</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="24"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="7" cm="1">
-        <f t="array" ref="H3:AE3">TRANSPOSE(C2:C25)</f>
-        <v>-11.9</v>
+        <f t="array" ref="H3:AE3">TRANSPOSE(B3:B26)</f>
+        <v>0</v>
       </c>
       <c r="I3" s="7">
-        <v>-5.6</v>
+        <v>0</v>
       </c>
       <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>0</v>
+      </c>
+      <c r="R3" s="7">
+        <v>0</v>
+      </c>
+      <c r="S3" s="7">
+        <v>0</v>
+      </c>
+      <c r="T3" s="7">
+        <v>0</v>
+      </c>
+      <c r="U3" s="7">
+        <v>0</v>
+      </c>
+      <c r="V3" s="7">
+        <v>0</v>
+      </c>
+      <c r="W3" s="7">
+        <v>0</v>
+      </c>
+      <c r="X3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="7">
         <v>-15.4</v>
       </c>
-      <c r="K3" s="7">
-        <v>14.6</v>
-      </c>
-      <c r="L3" s="7">
-        <v>-9.9</v>
-      </c>
-      <c r="M3" s="7">
-        <v>-7.1</v>
-      </c>
-      <c r="N3" s="7">
-        <v>-3.9</v>
-      </c>
-      <c r="O3" s="7">
-        <v>-6.3</v>
-      </c>
-      <c r="P3" s="7">
-        <v>-13.9</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>-9.3000000000000007</v>
-      </c>
-      <c r="R3" s="7">
-        <v>-9.8000000000000007</v>
-      </c>
-      <c r="S3" s="7">
-        <v>-3.3</v>
-      </c>
-      <c r="T3" s="7">
-        <v>-2</v>
-      </c>
-      <c r="U3" s="7">
-        <v>-10.7</v>
-      </c>
-      <c r="V3" s="7">
-        <v>-2.7</v>
-      </c>
-      <c r="W3" s="7">
-        <v>-7.8</v>
-      </c>
-      <c r="X3" s="7">
-        <v>3.3</v>
-      </c>
-      <c r="Y3" s="7">
-        <v>-4.5</v>
-      </c>
       <c r="Z3" s="7">
-        <v>-8.1</v>
+        <v>-18.8</v>
       </c>
       <c r="AA3" s="7">
-        <v>-15.8</v>
+        <v>-21.5</v>
       </c>
       <c r="AB3" s="7">
-        <v>-5.6</v>
+        <v>-26.1</v>
       </c>
       <c r="AC3" s="7">
-        <v>-11.7</v>
+        <v>-29.2</v>
       </c>
       <c r="AD3" s="7">
-        <v>-2.7</v>
+        <v>-17.7</v>
       </c>
       <c r="AE3" s="7">
-        <v>-16</v>
+        <v>-16.3</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="20">
-        <v>-26</v>
-      </c>
-      <c r="C4" s="20">
-        <v>-15.4</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="24"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
       <c r="G4" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="H4" s="7" cm="1">
+        <f t="array" ref="H4:AE4">TRANSPOSE(C3:C26)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0</v>
+      </c>
+      <c r="O4" s="7">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>0</v>
+      </c>
+      <c r="R4" s="7">
+        <v>0</v>
+      </c>
+      <c r="S4" s="7">
+        <v>0</v>
+      </c>
+      <c r="T4" s="7">
+        <v>0</v>
+      </c>
+      <c r="U4" s="7">
+        <v>0</v>
+      </c>
+      <c r="V4" s="7">
+        <v>0</v>
+      </c>
+      <c r="W4" s="7">
+        <v>0</v>
+      </c>
+      <c r="X4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="7">
+        <v>-6</v>
+      </c>
+      <c r="Z4" s="7">
+        <v>-11</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>-13</v>
+      </c>
+      <c r="AB4" s="7">
+        <v>-19.2</v>
+      </c>
+      <c r="AC4" s="7">
+        <v>-24.6</v>
+      </c>
+      <c r="AD4" s="7">
+        <v>-6.9</v>
+      </c>
+      <c r="AE4" s="7">
+        <v>-11.3</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="20">
-        <v>6.7</v>
-      </c>
-      <c r="C5" s="20">
-        <v>14.6</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="24"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="20">
-        <v>-17.2</v>
-      </c>
-      <c r="C6" s="20">
-        <v>-9.9</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="24"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="20">
-        <v>-14.3</v>
-      </c>
-      <c r="C7" s="20">
-        <v>-7.1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="20">
-        <v>-16</v>
-      </c>
-      <c r="C8" s="20">
-        <v>-3.9</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="24"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
@@ -1584,364 +1705,367 @@
     </row>
     <row r="9" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="20">
-        <v>-13.2</v>
-      </c>
-      <c r="C9" s="20">
-        <v>-6.3</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="24"/>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
       <c r="G9" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="20">
-        <v>-25.6</v>
-      </c>
-      <c r="C10" s="20">
-        <v>-13.9</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="24"/>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
       <c r="G10" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="20">
-        <v>-21.7</v>
-      </c>
-      <c r="C11" s="20">
-        <v>-9.3000000000000007</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="24"/>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
       <c r="G11" s="21" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="20">
-        <v>-19.2</v>
-      </c>
-      <c r="C12" s="20">
-        <v>-9.8000000000000007</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="24"/>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="20">
-        <v>-9.5</v>
-      </c>
-      <c r="C13" s="20">
-        <v>-3.3</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="24"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
       <c r="G13" s="21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="20">
-        <v>-9.6</v>
-      </c>
-      <c r="C14" s="20">
-        <v>-2</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="24"/>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
       <c r="G14" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="20">
-        <v>-26.9</v>
-      </c>
-      <c r="C15" s="20">
-        <v>-10.7</v>
-      </c>
-      <c r="D15" s="24">
-        <v>1</v>
-      </c>
-      <c r="E15" s="25">
-        <v>7</v>
-      </c>
-      <c r="F15" s="25">
-        <v>203</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="21" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="20">
-        <v>-11.7</v>
-      </c>
-      <c r="C16" s="20">
-        <v>-2.7</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="24">
         <v>1</v>
       </c>
       <c r="E16" s="25">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F16" s="25">
-        <v>212</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>67</v>
+        <v>203</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="20">
-        <v>-16.899999999999999</v>
-      </c>
-      <c r="C17" s="20">
-        <v>-7.8</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="24">
         <v>1</v>
       </c>
       <c r="E17" s="25">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F17" s="25">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="20">
-        <v>-12.7</v>
-      </c>
-      <c r="C18" s="20">
-        <v>3.3</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="24">
         <v>1</v>
       </c>
       <c r="E18" s="25">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="F18" s="25">
-        <v>292</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>88</v>
+        <v>225</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="20">
-        <v>-15.5</v>
-      </c>
-      <c r="C19" s="20">
-        <v>-4.5</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="24">
         <v>1</v>
       </c>
       <c r="E19" s="25">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="F19" s="25">
-        <v>211</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>67</v>
+        <v>292</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="27" t="s">
-        <v>68</v>
+      <c r="A20" s="40" t="s">
+        <v>47</v>
       </c>
       <c r="B20" s="20">
-        <v>-18</v>
+        <v>-15.4</v>
       </c>
       <c r="C20" s="20">
-        <v>-8.1</v>
+        <v>-6</v>
       </c>
       <c r="D20" s="24">
         <v>1</v>
       </c>
       <c r="E20" s="25">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F20" s="25">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="27" t="s">
-        <v>71</v>
+      <c r="A21" s="40" t="s">
+        <v>68</v>
       </c>
       <c r="B21" s="20">
-        <v>-20</v>
+        <v>-18.8</v>
       </c>
       <c r="C21" s="20">
-        <v>-15.8</v>
+        <v>-11</v>
       </c>
       <c r="D21" s="24">
         <v>1</v>
       </c>
       <c r="E21" s="25">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F21" s="25">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G21" s="22" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="27" t="s">
-        <v>76</v>
+      <c r="A22" s="40" t="s">
+        <v>71</v>
       </c>
       <c r="B22" s="20">
-        <v>-23.5</v>
-      </c>
-      <c r="C22" s="20">
-        <v>-5.6</v>
+        <v>-21.5</v>
+      </c>
+      <c r="C22" s="44">
+        <v>-13</v>
       </c>
       <c r="D22" s="24">
         <v>1</v>
       </c>
       <c r="E22" s="25">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F22" s="25">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="20">
-        <v>-25.5</v>
+      <c r="A23" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="44">
+        <v>-26.1</v>
       </c>
       <c r="C23" s="20">
-        <v>-11.7</v>
+        <v>-19.2</v>
       </c>
       <c r="D23" s="24">
         <v>1</v>
       </c>
       <c r="E23" s="25">
+        <v>45</v>
+      </c>
+      <c r="F23" s="25">
+        <v>243</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="20">
+        <v>-29.2</v>
+      </c>
+      <c r="C24" s="44">
+        <v>-24.6</v>
+      </c>
+      <c r="D24" s="24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="25">
         <v>72</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F24" s="25">
         <v>274</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G24" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="27" t="s">
+    <row r="25" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="20">
-        <v>-14.4</v>
-      </c>
-      <c r="C24" s="20">
-        <v>-2.7</v>
-      </c>
-      <c r="D24" s="24">
+      <c r="B25" s="20">
+        <v>-17.7</v>
+      </c>
+      <c r="C25" s="20">
+        <v>-6.9</v>
+      </c>
+      <c r="D25" s="24">
         <v>3</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E25" s="25">
         <v>77</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F25" s="25">
         <v>828</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G25" s="22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="27" t="s">
+    <row r="26" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="20">
-        <v>-24.1</v>
-      </c>
-      <c r="C25" s="20">
-        <v>-16</v>
-      </c>
-      <c r="D25" s="24">
+      <c r="B26" s="20">
+        <v>-16.3</v>
+      </c>
+      <c r="C26" s="20">
+        <v>-11.3</v>
+      </c>
+      <c r="D26" s="24">
         <v>4</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E26" s="25">
         <v>3</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F26" s="25">
         <v>893</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G26" s="22" t="s">
         <v>75</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="34">
+        <v>-33</v>
+      </c>
+      <c r="C28" s="33"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="34">
+        <v>-35.700000000000003</v>
+      </c>
+      <c r="C29" s="33"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="34">
+        <v>-35.700000000000003</v>
+      </c>
+      <c r="C30" s="33"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:G25">
-    <sortCondition ref="D19:D25"/>
-    <sortCondition ref="E19:E25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:G26">
+    <sortCondition ref="D20:D26"/>
+    <sortCondition ref="E20:E26"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1951,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF0FA41-85CC-443B-8D70-8487574C7D86}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1966,27 +2090,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="28"/>
+      <c r="A1" s="39"/>
       <c r="B1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="43.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="28"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+        <v>102</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="29" t="s">
         <v>96</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -2009,31 +2133,23 @@
       <c r="B4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="35">
-        <v>-27.5</v>
-      </c>
-      <c r="D4" s="35">
-        <v>-11.9</v>
-      </c>
-      <c r="E4" s="29" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="28" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15">
-        <v>14</v>
-      </c>
-      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="35">
-        <v>-26.9</v>
-      </c>
-      <c r="D5" s="35">
-        <v>-10.7</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>26</v>
+      <c r="B5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="28" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -2043,133 +2159,101 @@
       <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="35">
-        <v>-26</v>
-      </c>
-      <c r="D6" s="35">
-        <v>-15.4</v>
-      </c>
-      <c r="E6" s="29" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="28" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="15">
-        <v>9</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="35">
-        <v>-25.6</v>
-      </c>
-      <c r="D7" s="35">
-        <v>-13.9</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="15">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="35">
-        <v>-25.5</v>
-      </c>
-      <c r="D8" s="35">
-        <v>-11.7</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="28" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="15">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="35">
-        <v>-24.1</v>
-      </c>
-      <c r="D9" s="35">
-        <v>-16</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="28" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="15">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="28" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="35">
-        <v>-23.5</v>
-      </c>
-      <c r="D10" s="35">
-        <v>-5.6</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="15">
-        <v>2</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="35">
-        <v>-22.8</v>
-      </c>
-      <c r="D11" s="35">
-        <v>-5.6</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="28" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="15">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="35">
-        <v>-21.7</v>
-      </c>
-      <c r="D12" s="35">
-        <v>-9.3000000000000007</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>52</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="28" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="35">
-        <v>-20</v>
-      </c>
-      <c r="D13" s="35">
-        <v>-15.8</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="28" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
@@ -2179,235 +2263,179 @@
       <c r="B14" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="35">
-        <v>-19.2</v>
-      </c>
-      <c r="D14" s="35">
-        <v>-9.8000000000000007</v>
-      </c>
-      <c r="E14" s="29" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="35">
-        <v>-18</v>
-      </c>
-      <c r="D15" s="35">
-        <v>-8.1</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>28</v>
+        <v>58</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="28" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="15">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="35">
-        <v>-17.2</v>
-      </c>
-      <c r="D16" s="35">
-        <v>-9.9</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>23</v>
+        <v>62</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="28" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="35">
-        <v>-16.899999999999999</v>
-      </c>
-      <c r="D17" s="35">
-        <v>-7.8</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="28" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="15">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="35">
-        <v>-16</v>
-      </c>
-      <c r="D18" s="35">
-        <v>-3.9</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="15">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="35">
-        <v>-15.5</v>
-      </c>
-      <c r="D19" s="35">
-        <v>-4.5</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="28" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="15">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="35">
-        <v>-14.4</v>
-      </c>
-      <c r="D20" s="35">
-        <v>-2.7</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="28" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="15">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="35">
-        <v>-14.3</v>
-      </c>
-      <c r="D21" s="35">
-        <v>-7.1</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="15">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="35">
-        <v>-13.2</v>
-      </c>
-      <c r="D22" s="35">
-        <v>-6.3</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>22</v>
+        <v>69</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="28" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="15">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="35">
-        <v>-12.7</v>
-      </c>
-      <c r="D23" s="35">
-        <v>3.3</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>25</v>
+        <v>72</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="28" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="15">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="35">
-        <v>-11.7</v>
-      </c>
-      <c r="D24" s="35">
-        <v>-2.7</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>27</v>
+        <v>77</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="28" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="15">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="35">
-        <v>-9.6</v>
-      </c>
-      <c r="D25" s="35">
-        <v>-2</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="28" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="15">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="35">
-        <v>-9.5</v>
-      </c>
-      <c r="D26" s="35">
-        <v>-3.3</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="15">
-        <v>4</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="35">
-        <v>6.7</v>
-      </c>
-      <c r="D27" s="35">
-        <v>14.6</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="28" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
@@ -2439,7 +2467,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E27">
-    <sortCondition ref="C4:C27"/>
+    <sortCondition ref="A4:A27"/>
     <sortCondition ref="D4:D27"/>
   </sortState>
   <mergeCells count="2">
@@ -2530,7 +2558,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2772,6 +2800,78 @@
     <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4" s="17">
         <v>45612</v>
+      </c>
+      <c r="B4">
+        <v>-15.4</v>
+      </c>
+      <c r="C4">
+        <v>-18.5</v>
+      </c>
+      <c r="D4">
+        <v>-27.3</v>
+      </c>
+      <c r="E4">
+        <v>4.7</v>
+      </c>
+      <c r="F4">
+        <v>-21.1</v>
+      </c>
+      <c r="G4">
+        <v>-11.9</v>
+      </c>
+      <c r="H4">
+        <v>-10.9</v>
+      </c>
+      <c r="I4">
+        <v>-16.3</v>
+      </c>
+      <c r="J4">
+        <v>-16.5</v>
+      </c>
+      <c r="K4">
+        <v>-23.4</v>
+      </c>
+      <c r="L4">
+        <v>-15.6</v>
+      </c>
+      <c r="M4">
+        <v>-10.4</v>
+      </c>
+      <c r="N4">
+        <v>-8.6</v>
+      </c>
+      <c r="O4">
+        <v>-19.5</v>
+      </c>
+      <c r="P4">
+        <v>-12.4</v>
+      </c>
+      <c r="Q4">
+        <v>-22</v>
+      </c>
+      <c r="R4">
+        <v>-15.9</v>
+      </c>
+      <c r="S4">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="T4">
+        <v>-17.2</v>
+      </c>
+      <c r="U4">
+        <v>-22.6</v>
+      </c>
+      <c r="V4">
+        <v>-28.4</v>
+      </c>
+      <c r="W4">
+        <v>-27.9</v>
+      </c>
+      <c r="X4">
+        <v>-13.6</v>
+      </c>
+      <c r="Y4">
+        <v>-19</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.4">
@@ -2855,7 +2955,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2928,7 +3028,7 @@
         <v>71</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="W1" s="16" t="s">
         <v>46</v>
@@ -3097,6 +3197,78 @@
     <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4" s="17">
         <v>45612</v>
+      </c>
+      <c r="B4">
+        <v>-10.1</v>
+      </c>
+      <c r="C4">
+        <v>-7.8</v>
+      </c>
+      <c r="D4">
+        <v>-19</v>
+      </c>
+      <c r="E4">
+        <v>14.9</v>
+      </c>
+      <c r="F4">
+        <v>-8.6</v>
+      </c>
+      <c r="G4">
+        <v>-3.5</v>
+      </c>
+      <c r="H4">
+        <v>-2.4</v>
+      </c>
+      <c r="I4">
+        <v>-7.9</v>
+      </c>
+      <c r="J4">
+        <v>-11.7</v>
+      </c>
+      <c r="K4">
+        <v>-10.9</v>
+      </c>
+      <c r="L4">
+        <v>-8.1</v>
+      </c>
+      <c r="M4">
+        <v>-1.6</v>
+      </c>
+      <c r="N4">
+        <v>-1.8</v>
+      </c>
+      <c r="O4">
+        <v>-8.4</v>
+      </c>
+      <c r="P4">
+        <v>-0.7</v>
+      </c>
+      <c r="Q4">
+        <v>-6.4</v>
+      </c>
+      <c r="R4">
+        <v>-5.4</v>
+      </c>
+      <c r="S4">
+        <v>-1.2</v>
+      </c>
+      <c r="T4">
+        <v>-7</v>
+      </c>
+      <c r="U4">
+        <v>-6.4</v>
+      </c>
+      <c r="V4">
+        <v>-16.100000000000001</v>
+      </c>
+      <c r="W4">
+        <v>-14.5</v>
+      </c>
+      <c r="X4">
+        <v>-0.8</v>
+      </c>
+      <c r="Y4">
+        <v>-7.1</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.4">

</xml_diff>